<commit_message>
changing the order of if conditions for high scoring players
</commit_message>
<xml_diff>
--- a/nba_match_checker/today_matches_to_watch.xlsx
+++ b/nba_match_checker/today_matches_to_watch.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,72 +453,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pistons</t>
+          <t>Wizards</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hornets</t>
+          <t>Magic</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Warriors</t>
+          <t>Lakers</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pacers</t>
+          <t>Hawks</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hawks</t>
+          <t>Suns</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Magic</t>
+          <t>Raptors</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kings</t>
+          <t>Pistons</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Raptors</t>
+          <t>Bulls</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Knicks</t>
+          <t>Timberwolves</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bulls</t>
+          <t>Bucks</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -528,76 +528,61 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Heat</t>
+          <t>76ers</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Thunder</t>
+          <t>Pelicans</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Trail Blazers</t>
+          <t>Heat</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Spurs</t>
+          <t>Nuggets</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cavaliers</t>
+          <t>Trail Blazers</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mavericks</t>
+          <t>Warriors</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Wizards</t>
+          <t>Jazz</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Nuggets</t>
+          <t>Kings</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Timberwolves</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Clippers</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding selenium as an option for getting page source
</commit_message>
<xml_diff>
--- a/nba_match_checker/today_matches_to_watch.xlsx
+++ b/nba_match_checker/today_matches_to_watch.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,37 +453,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wizards</t>
+          <t>Cavaliers</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Magic</t>
+          <t>Hornets</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lakers</t>
+          <t>Pistons</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hawks</t>
+          <t>Wizards</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Suns</t>
+          <t>Nuggets</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -492,63 +492,63 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pistons</t>
+          <t>Lakers</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bulls</t>
+          <t>Pelicans</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Timberwolves</t>
+          <t>Nets</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bucks</t>
+          <t>Thunder</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>76ers</t>
+          <t>Magic</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Pelicans</t>
+          <t>Spurs</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Heat</t>
+          <t>Bucks</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nuggets</t>
+          <t>Suns</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -558,31 +558,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Knicks</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>Trail Blazers</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Warriors</t>
-        </is>
-      </c>
       <c r="C9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Jazz</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Kings</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>